<commit_message>
Aggiornamento test case applicativo PriamoRIS
Rieseguiti test [11,12] e aggiornati file data.json e report-checklist.xslx per l'applicativo PriamoRIS
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BCSSRL00000/BCS/PriamoRIS/4.14.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BCSSRL00000/BCS/PriamoRIS/4.14.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-fs01.bcs.it\shares\Rep-Software\A-FSE-2\Test Case\0 AAA VALIDAZIONE\1-Referto di Radiologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A6636E-97D7-4B2D-8983-DF404BEC37DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DAC6DB-7CDB-43CE-A779-82356C714B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3540" windowWidth="29040" windowHeight="15720" tabRatio="316" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="316" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -704,24 +704,6 @@
     <t>Il Modulo Priamo RIS include la sorica clinica in solo formato testuale a livello applicativo. Nel documento CDA2 viene quindi popolata la section relativa con la parte testuale. L'entry specifica richiesta dal test (ClinicalDocument/component/structuredBody/component/section[@ID=Storia_Clinica]/component/section[@ID=Allergie]/entry) non è quindi gestibile.</t>
   </si>
   <si>
-    <t>Thu, 16 Mar 2023 09:44:34 GMT</t>
-  </si>
-  <si>
-    <t>1e32e44396089bc0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6c52206b644043f09b41b3c74228843b4dfe48ebb8becb8da36c83ed0e434d10.4e3385a6e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Thu, 16 Mar 2023 10:00:47 GMT</t>
-  </si>
-  <si>
-    <t>b704d64836a2f0dd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6c52206b644043f09b41b3c74228843b4dfe48ebb8becb8da36c83ed0e434d10.6451e9807c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Thu, 16 Mar 2023 10:23:19 GMT</t>
   </si>
   <si>
@@ -729,6 +711,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6c52206b644043f09b41b3c74228843b4dfe48ebb8becb8da36c83ed0e434d10.793fa38c22^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e141b549f33da7ae</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6c52206b644043f09b41b3c74228843b4dfe48ebb8becb8da36c83ed0e434d10.cc98eb54b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Mon, 27 Mar 2023 11:55:01 GMT</t>
+  </si>
+  <si>
+    <t>Mon, 27 Mar 2023 11:57:02 GMT</t>
+  </si>
+  <si>
+    <t>089738612f943ae8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6c52206b644043f09b41b3c74228843b4dfe48ebb8becb8da36c83ed0e434d10.5e4149e4e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2687,10 +2687,10 @@
   <dimension ref="A1:O880"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2908,16 +2908,16 @@
         <v>29</v>
       </c>
       <c r="F10" s="17">
-        <v>45001</v>
+        <v>45012</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
@@ -2947,16 +2947,16 @@
         <v>31</v>
       </c>
       <c r="F11" s="17">
-        <v>45001</v>
+        <v>45012</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="37" t="s">
@@ -3207,13 +3207,13 @@
         <v>45001</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>118</v>

</xml_diff>